<commit_message>
Inverntory Data Cleaning and Analysis
</commit_message>
<xml_diff>
--- a/Formula Excel Template.xlsx
+++ b/Formula Excel Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Analysis\Excel\Playlist of Alex The Analyst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C419D55-53BC-44B7-A046-709B48FD7E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FCEEF1-8EA5-4419-86C9-BAEA93137BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="10" xr2:uid="{47981922-77C5-4EC3-A76E-98D6CE997DC2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="10" xr2:uid="{47981922-77C5-4EC3-A76E-98D6CE997DC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Max-Min" sheetId="9" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>

</xml_diff>